<commit_message>
Updated BGR_grids model - 2025-09-04 00:20
</commit_message>
<xml_diff>
--- a/VerveStacks_BGR_grids/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
+++ b/VerveStacks_BGR_grids/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_BGR_grids\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C88BCC5A-B433-4B21-9073-E4CFE8A0D1A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1EFFA4F8-E98E-4018-A44A-2179F01EF279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="8" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1364,18 +1364,72 @@
     <t>pre</t>
   </si>
   <si>
+    <t>distr_solelc_won-BGR_0011</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell BGR_11</t>
+  </si>
+  <si>
+    <t>NRGI</t>
+  </si>
+  <si>
+    <t>daynite</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-BGR_0022</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell BGR_22</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-BGR_0017</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell BGR_17</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-BGR_0013</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell BGR_13</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-BGR_0020</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell BGR_20</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-BGR_0046</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell BGR_46</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-BGR_0054</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell BGR_54</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-BGR_0037</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell BGR_37</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-BGR_0030</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell BGR_30</t>
+  </si>
+  <si>
     <t>distr_solelc_won-BGR_0023</t>
   </si>
   <si>
     <t>connecting solar and wind to buses in grid cell BGR_23</t>
   </si>
   <si>
-    <t>NRGI</t>
-  </si>
-  <si>
-    <t>daynite</t>
-  </si>
-  <si>
     <t>distr_solelc_won-BGR_0036</t>
   </si>
   <si>
@@ -1388,6 +1442,144 @@
     <t>connecting solar and wind to buses in grid cell BGR_56</t>
   </si>
   <si>
+    <t>distr_solelc_won-BGR_0014</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell BGR_14</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-BGR_0048</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell BGR_48</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-BGR_0035</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell BGR_35</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-BGR_0033</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell BGR_33</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-BGR_0045</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell BGR_45</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-BGR_0034</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell BGR_34</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-BGR_0040</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell BGR_40</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-BGR_0047</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell BGR_47</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-BGR_0052</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell BGR_52</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-BGR_0043</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell BGR_43</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-BGR_0031</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell BGR_31</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-BGR_0029</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell BGR_29</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-BGR_0039</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell BGR_39</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-BGR_0051</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell BGR_51</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-BGR_0055</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell BGR_55</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-BGR_0025</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell BGR_25</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-BGR_0006</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell BGR_6</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-BGR_0024</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell BGR_24</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-BGR_0038</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell BGR_38</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-BGR_0009</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell BGR_9</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-BGR_0015</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell BGR_15</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-BGR_0041</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell BGR_41</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-BGR_0049</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell BGR_49</t>
+  </si>
+  <si>
     <t>distr_solelc_won-BGR_0016</t>
   </si>
   <si>
@@ -1400,52 +1592,28 @@
     <t>connecting solar and wind to buses in grid cell BGR_2</t>
   </si>
   <si>
-    <t>distr_solelc_won-BGR_0037</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell BGR_37</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-BGR_0030</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell BGR_30</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-BGR_0033</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell BGR_33</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-BGR_0045</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell BGR_45</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-BGR_0034</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell BGR_34</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-BGR_0040</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell BGR_40</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-BGR_0047</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell BGR_47</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-BGR_0052</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell BGR_52</t>
+    <t>distr_solelc_won-BGR_0026</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell BGR_26</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-BGR_0027</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell BGR_27</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-BGR_0005</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell BGR_5</t>
+  </si>
+  <si>
+    <t>distr_solelc_won-BGR_0021</t>
+  </si>
+  <si>
+    <t>connecting solar and wind to buses in grid cell BGR_21</t>
   </si>
   <si>
     <t>distr_solelc_won-BGR_0044</t>
@@ -1472,90 +1640,6 @@
     <t>connecting solar and wind to buses in grid cell BGR_42</t>
   </si>
   <si>
-    <t>distr_solelc_won-BGR_0022</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell BGR_22</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-BGR_0017</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell BGR_17</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-BGR_0013</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell BGR_13</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-BGR_0020</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell BGR_20</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-BGR_0046</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell BGR_46</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-BGR_0054</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell BGR_54</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-BGR_0025</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell BGR_25</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-BGR_0006</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell BGR_6</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-BGR_0024</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell BGR_24</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-BGR_0038</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell BGR_38</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-BGR_0026</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell BGR_26</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-BGR_0027</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell BGR_27</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-BGR_0005</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell BGR_5</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-BGR_0021</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell BGR_21</t>
-  </si>
-  <si>
     <t>distr_solelc_won-BGR_0010</t>
   </si>
   <si>
@@ -1604,93 +1688,63 @@
     <t>connecting solar and wind to buses in grid cell BGR_28</t>
   </si>
   <si>
-    <t>distr_solelc_won-BGR_0014</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell BGR_14</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-BGR_0048</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell BGR_48</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-BGR_0035</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell BGR_35</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-BGR_0009</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell BGR_9</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-BGR_0015</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell BGR_15</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-BGR_0041</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell BGR_41</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-BGR_0049</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell BGR_49</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-BGR_0011</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell BGR_11</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-BGR_0043</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell BGR_43</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-BGR_0031</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell BGR_31</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-BGR_0029</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell BGR_29</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-BGR_0039</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell BGR_39</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-BGR_0051</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell BGR_51</t>
-  </si>
-  <si>
-    <t>distr_solelc_won-BGR_0055</t>
-  </si>
-  <si>
-    <t>connecting solar and wind to buses in grid cell BGR_55</t>
-  </si>
-  <si>
     <t>comm-in</t>
   </si>
   <si>
+    <t>elc_won-BGR_0011,elc_spv-BGR_0011</t>
+  </si>
+  <si>
+    <t>e_BG1-400,e_BG9-400</t>
+  </si>
+  <si>
+    <t>elc_won-BGR_0022,elc_spv-BGR_0022</t>
+  </si>
+  <si>
+    <t>e_BG14-220,e_w462198915-220</t>
+  </si>
+  <si>
+    <t>elc_won-BGR_0017,elc_spv-BGR_0017</t>
+  </si>
+  <si>
+    <t>e_BG2-220,e_BG3-220,e_BG3-400,e_BG4-400,e_BG5-400,e_BG6-400,e_BG7-400,e_BG8-400,e_w157471230-220,e_w157471230-400</t>
+  </si>
+  <si>
+    <t>elc_won-BGR_0013,elc_spv-BGR_0013</t>
+  </si>
+  <si>
+    <t>e_BG68-220,e_w1256110252-220,e_w243752614-400,e_w743367793-220,e_w743374599-400</t>
+  </si>
+  <si>
+    <t>elc_won-BGR_0020,elc_spv-BGR_0020</t>
+  </si>
+  <si>
+    <t>e_w96974919-400</t>
+  </si>
+  <si>
+    <t>elc_won-BGR_0046,elc_spv-BGR_0046</t>
+  </si>
+  <si>
+    <t>e_w259759898-220</t>
+  </si>
+  <si>
+    <t>elc_won-BGR_0054,elc_spv-BGR_0054</t>
+  </si>
+  <si>
+    <t>e_w261495737-220</t>
+  </si>
+  <si>
+    <t>elc_won-BGR_0037,elc_spv-BGR_0037</t>
+  </si>
+  <si>
+    <t>e_BG57-220,e_BG57-400,e_BG63-400,e_BG72-400</t>
+  </si>
+  <si>
+    <t>elc_won-BGR_0030,elc_spv-BGR_0030</t>
+  </si>
+  <si>
+    <t>e_BG72-400</t>
+  </si>
+  <si>
     <t>elc_won-BGR_0023,elc_spv-BGR_0023</t>
   </si>
   <si>
@@ -1700,15 +1754,120 @@
     <t>elc_won-BGR_0036,elc_spv-BGR_0036</t>
   </si>
   <si>
-    <t>e_BG72-400</t>
-  </si>
-  <si>
     <t>elc_won-BGR_0056,elc_spv-BGR_0056</t>
   </si>
   <si>
     <t>e_BG12-400</t>
   </si>
   <si>
+    <t>elc_won-BGR_0014,elc_spv-BGR_0014</t>
+  </si>
+  <si>
+    <t>e_w148478396-400</t>
+  </si>
+  <si>
+    <t>elc_won-BGR_0048,elc_spv-BGR_0048</t>
+  </si>
+  <si>
+    <t>e_w176754569-400</t>
+  </si>
+  <si>
+    <t>elc_won-BGR_0035,elc_spv-BGR_0035</t>
+  </si>
+  <si>
+    <t>e_w200514079-220</t>
+  </si>
+  <si>
+    <t>elc_won-BGR_0033,elc_spv-BGR_0033</t>
+  </si>
+  <si>
+    <t>e_BG21-220,e_BG22-220,e_BG23-220,e_BG24-220,e_BG25-220,e_BG38-220,e_BG39-220,e_w144024767-400</t>
+  </si>
+  <si>
+    <t>elc_won-BGR_0045,elc_spv-BGR_0045</t>
+  </si>
+  <si>
+    <t>elc_won-BGR_0034,elc_spv-BGR_0034</t>
+  </si>
+  <si>
+    <t>e_BG21-220</t>
+  </si>
+  <si>
+    <t>elc_won-BGR_0040,elc_spv-BGR_0040</t>
+  </si>
+  <si>
+    <t>elc_won-BGR_0047,elc_spv-BGR_0047</t>
+  </si>
+  <si>
+    <t>elc_won-BGR_0052,elc_spv-BGR_0052</t>
+  </si>
+  <si>
+    <t>elc_won-BGR_0043,elc_spv-BGR_0043</t>
+  </si>
+  <si>
+    <t>e_BG46-220,e_BG54-400,e_w178747356-220</t>
+  </si>
+  <si>
+    <t>elc_won-BGR_0031,elc_spv-BGR_0031</t>
+  </si>
+  <si>
+    <t>e_BG64-400,e_BG65-400,e_BG66-400,e_w1287693974-220,e_w1287693974-400,e_w157660797-220,e_w157660797-400,e_w253244460-400</t>
+  </si>
+  <si>
+    <t>elc_won-BGR_0029,elc_spv-BGR_0029</t>
+  </si>
+  <si>
+    <t>elc_won-BGR_0039,elc_spv-BGR_0039</t>
+  </si>
+  <si>
+    <t>e_BG39-220</t>
+  </si>
+  <si>
+    <t>elc_won-BGR_0051,elc_spv-BGR_0051</t>
+  </si>
+  <si>
+    <t>elc_won-BGR_0055,elc_spv-BGR_0055</t>
+  </si>
+  <si>
+    <t>elc_won-BGR_0025,elc_spv-BGR_0025</t>
+  </si>
+  <si>
+    <t>e_BG58-400</t>
+  </si>
+  <si>
+    <t>elc_won-BGR_0006,elc_spv-BGR_0006</t>
+  </si>
+  <si>
+    <t>e_w235044638-400</t>
+  </si>
+  <si>
+    <t>elc_won-BGR_0024,elc_spv-BGR_0024</t>
+  </si>
+  <si>
+    <t>elc_won-BGR_0038,elc_spv-BGR_0038</t>
+  </si>
+  <si>
+    <t>e_BG57-400</t>
+  </si>
+  <si>
+    <t>elc_won-BGR_0009,elc_spv-BGR_0009</t>
+  </si>
+  <si>
+    <t>e_BG26-400,e_BG27-400,e_BG28-400,e_BG29-400,e_BG32-400,e_BG33-400,e_BG34-400,e_BG35-400,e_BG36-400,e_BG37-400,e_BG40-220,e_BG41-220,e_BG42-220,e_w37028932-400,e_w37031469-220,e_w37031469-400</t>
+  </si>
+  <si>
+    <t>elc_won-BGR_0015,elc_spv-BGR_0015</t>
+  </si>
+  <si>
+    <t>elc_won-BGR_0041,elc_spv-BGR_0041</t>
+  </si>
+  <si>
+    <t>elc_won-BGR_0049,elc_spv-BGR_0049</t>
+  </si>
+  <si>
+    <t>e_BG20-400</t>
+  </si>
+  <si>
     <t>elc_won-BGR_0016,elc_spv-BGR_0016</t>
   </si>
   <si>
@@ -1721,46 +1880,28 @@
     <t>e_BG48-400,e_BG51-400,e_BG52-400,e_BG53-400,e_w176656979-400,e_w220458404-220</t>
   </si>
   <si>
-    <t>elc_won-BGR_0037,elc_spv-BGR_0037</t>
-  </si>
-  <si>
-    <t>e_BG57-220,e_BG57-400,e_BG63-400,e_BG72-400</t>
-  </si>
-  <si>
-    <t>elc_won-BGR_0030,elc_spv-BGR_0030</t>
-  </si>
-  <si>
-    <t>elc_won-BGR_0033,elc_spv-BGR_0033</t>
-  </si>
-  <si>
-    <t>e_BG21-220,e_BG22-220,e_BG23-220,e_BG24-220,e_BG25-220,e_BG38-220,e_BG39-220,e_w144024767-400</t>
-  </si>
-  <si>
-    <t>elc_won-BGR_0045,elc_spv-BGR_0045</t>
-  </si>
-  <si>
-    <t>e_w259759898-220</t>
-  </si>
-  <si>
-    <t>elc_won-BGR_0034,elc_spv-BGR_0034</t>
-  </si>
-  <si>
-    <t>e_BG21-220</t>
-  </si>
-  <si>
-    <t>elc_won-BGR_0040,elc_spv-BGR_0040</t>
-  </si>
-  <si>
-    <t>e_w200514079-220</t>
-  </si>
-  <si>
-    <t>elc_won-BGR_0047,elc_spv-BGR_0047</t>
-  </si>
-  <si>
-    <t>e_w176754569-400</t>
-  </si>
-  <si>
-    <t>elc_won-BGR_0052,elc_spv-BGR_0052</t>
+    <t>elc_won-BGR_0026,elc_spv-BGR_0026</t>
+  </si>
+  <si>
+    <t>e_BG47-220,e_BG49-220</t>
+  </si>
+  <si>
+    <t>elc_won-BGR_0027,elc_spv-BGR_0027</t>
+  </si>
+  <si>
+    <t>e_w262539285-220</t>
+  </si>
+  <si>
+    <t>elc_won-BGR_0005,elc_spv-BGR_0005</t>
+  </si>
+  <si>
+    <t>e_w232685942-220</t>
+  </si>
+  <si>
+    <t>elc_won-BGR_0021,elc_spv-BGR_0021</t>
+  </si>
+  <si>
+    <t>e_BG14-220</t>
   </si>
   <si>
     <t>elc_won-BGR_0044,elc_spv-BGR_0044</t>
@@ -1787,84 +1928,6 @@
     <t>e_BG54-400</t>
   </si>
   <si>
-    <t>elc_won-BGR_0022,elc_spv-BGR_0022</t>
-  </si>
-  <si>
-    <t>e_BG14-220,e_w462198915-220</t>
-  </si>
-  <si>
-    <t>elc_won-BGR_0017,elc_spv-BGR_0017</t>
-  </si>
-  <si>
-    <t>e_BG2-220,e_BG3-220,e_BG3-400,e_BG4-400,e_BG5-400,e_BG6-400,e_BG7-400,e_BG8-400,e_w157471230-220,e_w157471230-400</t>
-  </si>
-  <si>
-    <t>elc_won-BGR_0013,elc_spv-BGR_0013</t>
-  </si>
-  <si>
-    <t>e_BG68-220,e_w1256110252-220,e_w243752614-400,e_w743367793-220,e_w743374599-400</t>
-  </si>
-  <si>
-    <t>elc_won-BGR_0020,elc_spv-BGR_0020</t>
-  </si>
-  <si>
-    <t>e_w96974919-400</t>
-  </si>
-  <si>
-    <t>elc_won-BGR_0046,elc_spv-BGR_0046</t>
-  </si>
-  <si>
-    <t>elc_won-BGR_0054,elc_spv-BGR_0054</t>
-  </si>
-  <si>
-    <t>e_w261495737-220</t>
-  </si>
-  <si>
-    <t>elc_won-BGR_0025,elc_spv-BGR_0025</t>
-  </si>
-  <si>
-    <t>e_BG58-400</t>
-  </si>
-  <si>
-    <t>elc_won-BGR_0006,elc_spv-BGR_0006</t>
-  </si>
-  <si>
-    <t>e_w235044638-400</t>
-  </si>
-  <si>
-    <t>elc_won-BGR_0024,elc_spv-BGR_0024</t>
-  </si>
-  <si>
-    <t>elc_won-BGR_0038,elc_spv-BGR_0038</t>
-  </si>
-  <si>
-    <t>e_BG57-400</t>
-  </si>
-  <si>
-    <t>elc_won-BGR_0026,elc_spv-BGR_0026</t>
-  </si>
-  <si>
-    <t>e_BG47-220,e_BG49-220</t>
-  </si>
-  <si>
-    <t>elc_won-BGR_0027,elc_spv-BGR_0027</t>
-  </si>
-  <si>
-    <t>e_w262539285-220</t>
-  </si>
-  <si>
-    <t>elc_won-BGR_0005,elc_spv-BGR_0005</t>
-  </si>
-  <si>
-    <t>e_w232685942-220</t>
-  </si>
-  <si>
-    <t>elc_won-BGR_0021,elc_spv-BGR_0021</t>
-  </si>
-  <si>
-    <t>e_BG14-220</t>
-  </si>
-  <si>
     <t>elc_won-BGR_0010,elc_spv-BGR_0010</t>
   </si>
   <si>
@@ -1905,69 +1968,6 @@
   </si>
   <si>
     <t>e_w144024767-400</t>
-  </si>
-  <si>
-    <t>elc_won-BGR_0014,elc_spv-BGR_0014</t>
-  </si>
-  <si>
-    <t>e_w148478396-400</t>
-  </si>
-  <si>
-    <t>elc_won-BGR_0048,elc_spv-BGR_0048</t>
-  </si>
-  <si>
-    <t>elc_won-BGR_0035,elc_spv-BGR_0035</t>
-  </si>
-  <si>
-    <t>elc_won-BGR_0009,elc_spv-BGR_0009</t>
-  </si>
-  <si>
-    <t>e_BG26-400,e_BG27-400,e_BG28-400,e_BG29-400,e_BG32-400,e_BG33-400,e_BG34-400,e_BG35-400,e_BG36-400,e_BG37-400,e_BG40-220,e_BG41-220,e_BG42-220,e_w37028932-400,e_w37031469-220,e_w37031469-400</t>
-  </si>
-  <si>
-    <t>elc_won-BGR_0015,elc_spv-BGR_0015</t>
-  </si>
-  <si>
-    <t>elc_won-BGR_0041,elc_spv-BGR_0041</t>
-  </si>
-  <si>
-    <t>elc_won-BGR_0049,elc_spv-BGR_0049</t>
-  </si>
-  <si>
-    <t>e_BG20-400</t>
-  </si>
-  <si>
-    <t>elc_won-BGR_0011,elc_spv-BGR_0011</t>
-  </si>
-  <si>
-    <t>e_BG1-400,e_BG9-400</t>
-  </si>
-  <si>
-    <t>elc_won-BGR_0043,elc_spv-BGR_0043</t>
-  </si>
-  <si>
-    <t>e_BG46-220,e_BG54-400,e_w178747356-220</t>
-  </si>
-  <si>
-    <t>elc_won-BGR_0031,elc_spv-BGR_0031</t>
-  </si>
-  <si>
-    <t>e_BG64-400,e_BG65-400,e_BG66-400,e_w1287693974-220,e_w1287693974-400,e_w157660797-220,e_w157660797-400,e_w253244460-400</t>
-  </si>
-  <si>
-    <t>elc_won-BGR_0029,elc_spv-BGR_0029</t>
-  </si>
-  <si>
-    <t>elc_won-BGR_0039,elc_spv-BGR_0039</t>
-  </si>
-  <si>
-    <t>e_BG39-220</t>
-  </si>
-  <si>
-    <t>elc_won-BGR_0051,elc_spv-BGR_0051</t>
-  </si>
-  <si>
-    <t>elc_won-BGR_0055,elc_spv-BGR_0055</t>
   </si>
   <si>
     <t>e_won-BGR_0000</t>
@@ -7741,7 +7741,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{304AAB1A-BD62-4D5A-B62A-307B397C8562}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57C25140-CEEA-45AD-8BC9-F89B52F15D66}">
   <dimension ref="B9:AC65"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -7913,7 +7913,7 @@
         <v>1</v>
       </c>
       <c r="AC11" t="s">
-        <v>343</v>
+        <v>321</v>
       </c>
     </row>
     <row r="12" spans="2:29">
@@ -7990,7 +7990,7 @@
         <v>1</v>
       </c>
       <c r="AC12" t="s">
-        <v>369</v>
+        <v>341</v>
       </c>
     </row>
     <row r="13" spans="2:29">
@@ -8067,7 +8067,7 @@
         <v>1</v>
       </c>
       <c r="AC13" t="s">
-        <v>407</v>
+        <v>333</v>
       </c>
     </row>
     <row r="14" spans="2:29">
@@ -8144,7 +8144,7 @@
         <v>1</v>
       </c>
       <c r="AC14" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
     </row>
     <row r="15" spans="2:29">
@@ -8221,7 +8221,7 @@
         <v>1</v>
       </c>
       <c r="AC15" t="s">
-        <v>303</v>
+        <v>337</v>
       </c>
     </row>
     <row r="16" spans="2:29">
@@ -8298,7 +8298,7 @@
         <v>1</v>
       </c>
       <c r="AC16" t="s">
-        <v>371</v>
+        <v>389</v>
       </c>
     </row>
     <row r="17" spans="2:29">
@@ -8369,13 +8369,13 @@
         <v>532</v>
       </c>
       <c r="AA17" t="s">
-        <v>523</v>
+        <v>533</v>
       </c>
       <c r="AB17">
         <v>1</v>
       </c>
       <c r="AC17" t="s">
-        <v>357</v>
+        <v>403</v>
       </c>
     </row>
     <row r="18" spans="2:29">
@@ -8443,16 +8443,16 @@
         <v>427</v>
       </c>
       <c r="Z18" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="AA18" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="AB18">
         <v>1</v>
       </c>
       <c r="AC18" t="s">
-        <v>363</v>
+        <v>371</v>
       </c>
     </row>
     <row r="19" spans="2:29">
@@ -8520,16 +8520,16 @@
         <v>429</v>
       </c>
       <c r="Z19" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="AA19" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="AB19">
         <v>1</v>
       </c>
       <c r="AC19" t="s">
-        <v>387</v>
+        <v>357</v>
       </c>
     </row>
     <row r="20" spans="2:29">
@@ -8597,16 +8597,16 @@
         <v>431</v>
       </c>
       <c r="Z20" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="AA20" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="AB20">
         <v>1</v>
       </c>
       <c r="AC20" t="s">
-        <v>365</v>
+        <v>343</v>
       </c>
     </row>
     <row r="21" spans="2:29">
@@ -8674,16 +8674,16 @@
         <v>433</v>
       </c>
       <c r="Z21" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="AA21" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="AB21">
         <v>1</v>
       </c>
       <c r="AC21" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
     </row>
     <row r="22" spans="2:29">
@@ -8760,7 +8760,7 @@
         <v>1</v>
       </c>
       <c r="AC22" t="s">
-        <v>391</v>
+        <v>407</v>
       </c>
     </row>
     <row r="23" spans="2:29">
@@ -8831,13 +8831,13 @@
         <v>543</v>
       </c>
       <c r="AA23" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="AB23">
         <v>1</v>
       </c>
       <c r="AC23" t="s">
-        <v>401</v>
+        <v>327</v>
       </c>
     </row>
     <row r="24" spans="2:29">
@@ -8905,16 +8905,16 @@
         <v>439</v>
       </c>
       <c r="Z24" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="AA24" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="AB24">
         <v>1</v>
       </c>
       <c r="AC24" t="s">
-        <v>385</v>
+        <v>393</v>
       </c>
     </row>
     <row r="25" spans="2:29">
@@ -8982,16 +8982,16 @@
         <v>441</v>
       </c>
       <c r="Z25" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="AA25" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="AB25">
         <v>1</v>
       </c>
       <c r="AC25" t="s">
-        <v>361</v>
+        <v>367</v>
       </c>
     </row>
     <row r="26" spans="2:29">
@@ -9059,16 +9059,16 @@
         <v>443</v>
       </c>
       <c r="Z26" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="AA26" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="AB26">
         <v>1</v>
       </c>
       <c r="AC26" t="s">
-        <v>301</v>
+        <v>363</v>
       </c>
     </row>
     <row r="27" spans="2:29">
@@ -9136,16 +9136,16 @@
         <v>445</v>
       </c>
       <c r="Z27" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="AA27" t="s">
-        <v>551</v>
+        <v>531</v>
       </c>
       <c r="AB27">
         <v>1</v>
       </c>
       <c r="AC27" t="s">
-        <v>381</v>
+        <v>387</v>
       </c>
     </row>
     <row r="28" spans="2:29">
@@ -9222,7 +9222,7 @@
         <v>1</v>
       </c>
       <c r="AC28" t="s">
-        <v>341</v>
+        <v>365</v>
       </c>
     </row>
     <row r="29" spans="2:29">
@@ -9293,13 +9293,13 @@
         <v>554</v>
       </c>
       <c r="AA29" t="s">
-        <v>555</v>
+        <v>548</v>
       </c>
       <c r="AB29">
         <v>1</v>
       </c>
       <c r="AC29" t="s">
-        <v>333</v>
+        <v>377</v>
       </c>
     </row>
     <row r="30" spans="2:29">
@@ -9367,16 +9367,16 @@
         <v>451</v>
       </c>
       <c r="Z30" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="AA30" t="s">
-        <v>557</v>
+        <v>546</v>
       </c>
       <c r="AB30">
         <v>1</v>
       </c>
       <c r="AC30" t="s">
-        <v>325</v>
+        <v>391</v>
       </c>
     </row>
     <row r="31" spans="2:29">
@@ -9444,16 +9444,16 @@
         <v>453</v>
       </c>
       <c r="Z31" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="AA31" t="s">
-        <v>559</v>
+        <v>546</v>
       </c>
       <c r="AB31">
         <v>1</v>
       </c>
       <c r="AC31" t="s">
-        <v>337</v>
+        <v>401</v>
       </c>
     </row>
     <row r="32" spans="2:29">
@@ -9521,16 +9521,16 @@
         <v>455</v>
       </c>
       <c r="Z32" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="AA32" t="s">
-        <v>536</v>
+        <v>558</v>
       </c>
       <c r="AB32">
         <v>1</v>
       </c>
       <c r="AC32" t="s">
-        <v>389</v>
+        <v>383</v>
       </c>
     </row>
     <row r="33" spans="2:29">
@@ -9598,16 +9598,16 @@
         <v>457</v>
       </c>
       <c r="Z33" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="AA33" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="AB33">
         <v>1</v>
       </c>
       <c r="AC33" t="s">
-        <v>403</v>
+        <v>359</v>
       </c>
     </row>
     <row r="34" spans="2:29">
@@ -9675,16 +9675,16 @@
         <v>459</v>
       </c>
       <c r="Z34" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="AA34" t="s">
-        <v>564</v>
+        <v>539</v>
       </c>
       <c r="AB34">
         <v>1</v>
       </c>
       <c r="AC34" t="s">
-        <v>347</v>
+        <v>355</v>
       </c>
     </row>
     <row r="35" spans="2:29">
@@ -9752,16 +9752,16 @@
         <v>461</v>
       </c>
       <c r="Z35" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="AA35" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="AB35">
         <v>1</v>
       </c>
       <c r="AC35" t="s">
-        <v>311</v>
+        <v>375</v>
       </c>
     </row>
     <row r="36" spans="2:29">
@@ -9829,16 +9829,16 @@
         <v>463</v>
       </c>
       <c r="Z36" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="AA36" t="s">
-        <v>559</v>
+        <v>542</v>
       </c>
       <c r="AB36">
         <v>1</v>
       </c>
       <c r="AC36" t="s">
-        <v>345</v>
+        <v>399</v>
       </c>
     </row>
     <row r="37" spans="2:29">
@@ -9906,16 +9906,16 @@
         <v>465</v>
       </c>
       <c r="Z37" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="AA37" t="s">
-        <v>569</v>
+        <v>533</v>
       </c>
       <c r="AB37">
         <v>1</v>
       </c>
       <c r="AC37" t="s">
-        <v>373</v>
+        <v>405</v>
       </c>
     </row>
     <row r="38" spans="2:29">
@@ -9983,16 +9983,16 @@
         <v>467</v>
       </c>
       <c r="Z38" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
       <c r="AA38" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
       <c r="AB38">
         <v>1</v>
       </c>
       <c r="AC38" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="39" spans="2:29">
@@ -10060,16 +10060,16 @@
         <v>469</v>
       </c>
       <c r="Z39" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="AA39" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="AB39">
         <v>1</v>
       </c>
       <c r="AC39" t="s">
-        <v>351</v>
+        <v>311</v>
       </c>
     </row>
     <row r="40" spans="2:29">
@@ -10137,16 +10137,16 @@
         <v>471</v>
       </c>
       <c r="Z40" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
       <c r="AA40" t="s">
-        <v>575</v>
+        <v>529</v>
       </c>
       <c r="AB40">
         <v>1</v>
       </c>
       <c r="AC40" t="s">
-        <v>309</v>
+        <v>345</v>
       </c>
     </row>
     <row r="41" spans="2:29">
@@ -10214,16 +10214,16 @@
         <v>473</v>
       </c>
       <c r="Z41" t="s">
-        <v>576</v>
+        <v>571</v>
       </c>
       <c r="AA41" t="s">
-        <v>577</v>
+        <v>572</v>
       </c>
       <c r="AB41">
         <v>1</v>
       </c>
       <c r="AC41" t="s">
-        <v>339</v>
+        <v>373</v>
       </c>
     </row>
     <row r="42" spans="2:29">
@@ -10291,16 +10291,16 @@
         <v>475</v>
       </c>
       <c r="Z42" t="s">
-        <v>578</v>
+        <v>573</v>
       </c>
       <c r="AA42" t="s">
-        <v>579</v>
+        <v>574</v>
       </c>
       <c r="AB42">
         <v>1</v>
       </c>
       <c r="AC42" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="43" spans="2:29">
@@ -10368,16 +10368,16 @@
         <v>477</v>
       </c>
       <c r="Z43" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="AA43" t="s">
-        <v>581</v>
+        <v>544</v>
       </c>
       <c r="AB43">
         <v>1</v>
       </c>
       <c r="AC43" t="s">
-        <v>397</v>
+        <v>329</v>
       </c>
     </row>
     <row r="44" spans="2:29">
@@ -10445,16 +10445,16 @@
         <v>479</v>
       </c>
       <c r="Z44" t="s">
-        <v>582</v>
+        <v>576</v>
       </c>
       <c r="AA44" t="s">
-        <v>583</v>
+        <v>548</v>
       </c>
       <c r="AB44">
         <v>1</v>
       </c>
       <c r="AC44" t="s">
-        <v>315</v>
+        <v>379</v>
       </c>
     </row>
     <row r="45" spans="2:29">
@@ -10522,16 +10522,16 @@
         <v>481</v>
       </c>
       <c r="Z45" t="s">
-        <v>584</v>
+        <v>577</v>
       </c>
       <c r="AA45" t="s">
-        <v>566</v>
+        <v>578</v>
       </c>
       <c r="AB45">
         <v>1</v>
       </c>
       <c r="AC45" t="s">
-        <v>313</v>
+        <v>395</v>
       </c>
     </row>
     <row r="46" spans="2:29">
@@ -10599,16 +10599,16 @@
         <v>483</v>
       </c>
       <c r="Z46" t="s">
-        <v>585</v>
+        <v>579</v>
       </c>
       <c r="AA46" t="s">
-        <v>566</v>
+        <v>580</v>
       </c>
       <c r="AB46">
         <v>1</v>
       </c>
       <c r="AC46" t="s">
-        <v>299</v>
+        <v>331</v>
       </c>
     </row>
     <row r="47" spans="2:29">
@@ -10676,16 +10676,16 @@
         <v>485</v>
       </c>
       <c r="Z47" t="s">
-        <v>586</v>
+        <v>581</v>
       </c>
       <c r="AA47" t="s">
-        <v>587</v>
+        <v>582</v>
       </c>
       <c r="AB47">
         <v>1</v>
       </c>
       <c r="AC47" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="48" spans="2:29">
@@ -10753,16 +10753,16 @@
         <v>487</v>
       </c>
       <c r="Z48" t="s">
-        <v>588</v>
+        <v>583</v>
       </c>
       <c r="AA48" t="s">
-        <v>589</v>
+        <v>584</v>
       </c>
       <c r="AB48">
         <v>1</v>
       </c>
       <c r="AC48" t="s">
-        <v>307</v>
+        <v>349</v>
       </c>
     </row>
     <row r="49" spans="2:29">
@@ -10830,16 +10830,16 @@
         <v>489</v>
       </c>
       <c r="Z49" t="s">
-        <v>590</v>
+        <v>585</v>
       </c>
       <c r="AA49" t="s">
-        <v>591</v>
+        <v>586</v>
       </c>
       <c r="AB49">
         <v>1</v>
       </c>
       <c r="AC49" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="50" spans="2:29">
@@ -10907,16 +10907,16 @@
         <v>491</v>
       </c>
       <c r="Z50" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
       <c r="AA50" t="s">
-        <v>593</v>
+        <v>588</v>
       </c>
       <c r="AB50">
         <v>1</v>
       </c>
       <c r="AC50" t="s">
-        <v>327</v>
+        <v>309</v>
       </c>
     </row>
     <row r="51" spans="2:29">
@@ -10984,16 +10984,16 @@
         <v>493</v>
       </c>
       <c r="Z51" t="s">
-        <v>594</v>
+        <v>589</v>
       </c>
       <c r="AA51" t="s">
-        <v>542</v>
+        <v>590</v>
       </c>
       <c r="AB51">
         <v>1</v>
       </c>
       <c r="AC51" t="s">
-        <v>393</v>
+        <v>339</v>
       </c>
     </row>
     <row r="52" spans="2:29">
@@ -11061,16 +11061,16 @@
         <v>495</v>
       </c>
       <c r="Z52" t="s">
-        <v>595</v>
+        <v>591</v>
       </c>
       <c r="AA52" t="s">
-        <v>540</v>
+        <v>592</v>
       </c>
       <c r="AB52">
         <v>1</v>
       </c>
       <c r="AC52" t="s">
-        <v>367</v>
+        <v>385</v>
       </c>
     </row>
     <row r="53" spans="2:29">
@@ -11138,16 +11138,16 @@
         <v>497</v>
       </c>
       <c r="Z53" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="AA53" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="AB53">
         <v>1</v>
       </c>
       <c r="AC53" t="s">
-        <v>317</v>
+        <v>361</v>
       </c>
     </row>
     <row r="54" spans="2:29">
@@ -11215,16 +11215,16 @@
         <v>499</v>
       </c>
       <c r="Z54" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="AA54" t="s">
-        <v>593</v>
+        <v>596</v>
       </c>
       <c r="AB54">
         <v>1</v>
       </c>
       <c r="AC54" t="s">
-        <v>329</v>
+        <v>301</v>
       </c>
     </row>
     <row r="55" spans="2:29">
@@ -11292,16 +11292,16 @@
         <v>501</v>
       </c>
       <c r="Z55" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="AA55" t="s">
-        <v>540</v>
+        <v>598</v>
       </c>
       <c r="AB55">
         <v>1</v>
       </c>
       <c r="AC55" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
     </row>
     <row r="56" spans="2:29">
@@ -11369,16 +11369,16 @@
         <v>503</v>
       </c>
       <c r="Z56" t="s">
+        <v>599</v>
+      </c>
+      <c r="AA56" t="s">
         <v>600</v>
-      </c>
-      <c r="AA56" t="s">
-        <v>601</v>
       </c>
       <c r="AB56">
         <v>1</v>
       </c>
       <c r="AC56" t="s">
-        <v>395</v>
+        <v>319</v>
       </c>
     </row>
     <row r="57" spans="2:29">
@@ -11446,16 +11446,16 @@
         <v>505</v>
       </c>
       <c r="Z57" t="s">
+        <v>601</v>
+      </c>
+      <c r="AA57" t="s">
         <v>602</v>
-      </c>
-      <c r="AA57" t="s">
-        <v>603</v>
       </c>
       <c r="AB57">
         <v>1</v>
       </c>
       <c r="AC57" t="s">
-        <v>321</v>
+        <v>397</v>
       </c>
     </row>
     <row r="58" spans="2:29">
@@ -11523,16 +11523,16 @@
         <v>507</v>
       </c>
       <c r="Z58" t="s">
+        <v>603</v>
+      </c>
+      <c r="AA58" t="s">
         <v>604</v>
-      </c>
-      <c r="AA58" t="s">
-        <v>605</v>
       </c>
       <c r="AB58">
         <v>1</v>
       </c>
       <c r="AC58" t="s">
-        <v>383</v>
+        <v>315</v>
       </c>
     </row>
     <row r="59" spans="2:29">
@@ -11600,16 +11600,16 @@
         <v>509</v>
       </c>
       <c r="Z59" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="AA59" t="s">
-        <v>607</v>
+        <v>569</v>
       </c>
       <c r="AB59">
         <v>1</v>
       </c>
       <c r="AC59" t="s">
-        <v>359</v>
+        <v>313</v>
       </c>
     </row>
     <row r="60" spans="2:29">
@@ -11677,16 +11677,16 @@
         <v>511</v>
       </c>
       <c r="Z60" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="AA60" t="s">
-        <v>521</v>
+        <v>569</v>
       </c>
       <c r="AB60">
         <v>1</v>
       </c>
       <c r="AC60" t="s">
-        <v>355</v>
+        <v>299</v>
       </c>
     </row>
     <row r="61" spans="2:29">
@@ -11754,16 +11754,16 @@
         <v>513</v>
       </c>
       <c r="Z61" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="AA61" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="AB61">
         <v>1</v>
       </c>
       <c r="AC61" t="s">
-        <v>375</v>
+        <v>305</v>
       </c>
     </row>
     <row r="62" spans="2:29">
@@ -11831,16 +11831,16 @@
         <v>515</v>
       </c>
       <c r="Z62" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="AA62" t="s">
-        <v>525</v>
+        <v>610</v>
       </c>
       <c r="AB62">
         <v>1</v>
       </c>
       <c r="AC62" t="s">
-        <v>399</v>
+        <v>307</v>
       </c>
     </row>
     <row r="63" spans="2:29">
@@ -11908,16 +11908,16 @@
         <v>517</v>
       </c>
       <c r="Z63" t="s">
+        <v>611</v>
+      </c>
+      <c r="AA63" t="s">
         <v>612</v>
-      </c>
-      <c r="AA63" t="s">
-        <v>562</v>
       </c>
       <c r="AB63">
         <v>1</v>
       </c>
       <c r="AC63" t="s">
-        <v>405</v>
+        <v>353</v>
       </c>
     </row>
     <row r="64" spans="2:29">
@@ -12002,7 +12002,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DE88012-8184-41A3-9B05-77E90A22693E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0489FFDA-CDDC-40F5-A8CF-42CC15CAB5A4}">
   <dimension ref="B9:AB65"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -14805,7 +14805,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59E37C0C-EB88-4C89-B582-8FF6758BF4C3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A346C417-6805-4812-9C4E-D8FE4548AC4F}">
   <dimension ref="B9:P73"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -16625,7 +16625,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFF32174-F703-4FBB-878E-BB267CB4FF79}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{310F3FEB-4BB7-4DF2-B917-C3E4059FC4BD}">
   <dimension ref="B2:M27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -16805,7 +16805,7 @@
         <v>846</v>
       </c>
       <c r="C8" t="s">
-        <v>569</v>
+        <v>572</v>
       </c>
       <c r="D8" t="s">
         <v>847</v>
@@ -16840,7 +16840,7 @@
         <v>847</v>
       </c>
       <c r="D9" t="s">
-        <v>569</v>
+        <v>572</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -17381,7 +17381,7 @@
         <v>881</v>
       </c>
       <c r="C26" t="s">
-        <v>559</v>
+        <v>529</v>
       </c>
       <c r="D26" t="s">
         <v>882</v>
@@ -17416,7 +17416,7 @@
         <v>882</v>
       </c>
       <c r="D27" t="s">
-        <v>559</v>
+        <v>529</v>
       </c>
       <c r="E27">
         <v>1</v>

</xml_diff>